<commit_message>
Fixed calculations and status table
</commit_message>
<xml_diff>
--- a/csv_data_files/Tech Report.xlsx
+++ b/csv_data_files/Tech Report.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/e2073ff4a448c905/Documents/Python Projects/Reliability Dashboard/csv_data_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="333" documentId="11_F25DC773A252ABDACC1048C5811E4E1A5BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BB15D268-86C8-4741-9325-13169D0CB793}"/>
+  <xr:revisionPtr revIDLastSave="334" documentId="11_F25DC773A252ABDACC1048C5811E4E1A5BDE58F0" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2E4DFD69-A3AA-47CF-BEF8-88DCD1B26A59}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="UTIL" sheetId="2" r:id="rId1"/>
@@ -333,10 +333,10 @@
   </cellStyles>
   <dxfs count="5">
     <dxf>
-      <numFmt numFmtId="14" formatCode="0.00%"/>
+      <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
+      <numFmt numFmtId="14" formatCode="0.00%"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
@@ -6862,6 +6862,131 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90FEFAF0-372C-4C34-AC9C-A0EF7D794D17}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="O2:R13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="12">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" numFmtId="164" showAll="0">
+      <items count="13">
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="9"/>
+        <item x="10"/>
+        <item x="11"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField dataField="1" numFmtId="9" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="4"/>
+  </rowFields>
+  <rowItems count="11">
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="-2"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i i="1">
+      <x v="1"/>
+    </i>
+    <i i="2">
+      <x v="2"/>
+    </i>
+  </colItems>
+  <dataFields count="3">
+    <dataField name="Sum of CYC" fld="3" baseField="0" baseItem="0"/>
+    <dataField name="Sum of DELAY" fld="8" baseField="0" baseItem="0"/>
+    <dataField name="Average of DR" fld="9" subtotal="average" baseField="4" baseItem="3"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="2">
+          <reference field="4294967294" count="1" selected="0">
+            <x v="2"/>
+          </reference>
+          <reference field="4" count="10">
+            <x v="1"/>
+            <x v="2"/>
+            <x v="3"/>
+            <x v="4"/>
+            <x v="5"/>
+            <x v="6"/>
+            <x v="7"/>
+            <x v="8"/>
+            <x v="9"/>
+            <x v="10"/>
+          </reference>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
+      <xpdl:pivotTableDefinition16/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{1B6B77EB-D272-4363-83FF-33F3EF9D3DE6}" name="PivotTable11" cacheId="2" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O22:S24" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="14">
@@ -7018,7 +7143,7 @@
     <dataField name="Sum of FL_DURR" fld="12" baseField="4" baseItem="1"/>
   </dataFields>
   <formats count="1">
-    <format dxfId="0">
+    <format dxfId="1">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -7043,7 +7168,7 @@
 </pivotTableDefinition>
 </file>
 
-<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{842CC2E9-9555-4F18-BE60-0BFA0A2428D2}" name="PivotTable9" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="O16:R20" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="11">
@@ -7487,7 +7612,7 @@
     <dataField name="Average of DR" fld="9" subtotal="average" baseField="10" baseItem="4"/>
   </dataFields>
   <formats count="3">
-    <format dxfId="3">
+    <format dxfId="4">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -7499,7 +7624,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="2">
+    <format dxfId="3">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -7511,7 +7636,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="1">
+    <format dxfId="2">
       <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
         <references count="2">
           <reference field="4294967294" count="1" selected="0">
@@ -7519,131 +7644,6 @@
           </reference>
           <reference field="10" count="1">
             <x v="6"/>
-          </reference>
-        </references>
-      </pivotArea>
-    </format>
-  </formats>
-  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
-      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
-    </ext>
-    <ext xmlns:xpdl="http://schemas.microsoft.com/office/spreadsheetml/2016/pivotdefaultlayout" uri="{747A6164-185A-40DC-8AA5-F01512510D54}">
-      <xpdl:pivotTableDefinition16/>
-    </ext>
-  </extLst>
-</pivotTableDefinition>
-</file>
-
-<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{90FEFAF0-372C-4C34-AC9C-A0EF7D794D17}" name="PivotTable2" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="O2:R13" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
-  <pivotFields count="12">
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField axis="axisRow" numFmtId="164" showAll="0">
-      <items count="13">
-        <item x="0"/>
-        <item x="1"/>
-        <item x="2"/>
-        <item x="3"/>
-        <item x="4"/>
-        <item x="5"/>
-        <item x="6"/>
-        <item x="7"/>
-        <item x="8"/>
-        <item x="9"/>
-        <item x="10"/>
-        <item x="11"/>
-        <item t="default"/>
-      </items>
-    </pivotField>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField dataField="1" showAll="0"/>
-    <pivotField dataField="1" numFmtId="9" showAll="0"/>
-    <pivotField showAll="0"/>
-    <pivotField showAll="0"/>
-  </pivotFields>
-  <rowFields count="1">
-    <field x="4"/>
-  </rowFields>
-  <rowItems count="11">
-    <i>
-      <x v="1"/>
-    </i>
-    <i>
-      <x v="2"/>
-    </i>
-    <i>
-      <x v="3"/>
-    </i>
-    <i>
-      <x v="4"/>
-    </i>
-    <i>
-      <x v="5"/>
-    </i>
-    <i>
-      <x v="6"/>
-    </i>
-    <i>
-      <x v="7"/>
-    </i>
-    <i>
-      <x v="8"/>
-    </i>
-    <i>
-      <x v="9"/>
-    </i>
-    <i>
-      <x v="10"/>
-    </i>
-    <i t="grand">
-      <x/>
-    </i>
-  </rowItems>
-  <colFields count="1">
-    <field x="-2"/>
-  </colFields>
-  <colItems count="3">
-    <i>
-      <x/>
-    </i>
-    <i i="1">
-      <x v="1"/>
-    </i>
-    <i i="2">
-      <x v="2"/>
-    </i>
-  </colItems>
-  <dataFields count="3">
-    <dataField name="Sum of CYC" fld="3" baseField="0" baseItem="0"/>
-    <dataField name="Sum of DELAY" fld="8" baseField="0" baseItem="0"/>
-    <dataField name="Average of DR" fld="9" subtotal="average" baseField="4" baseItem="3"/>
-  </dataFields>
-  <formats count="1">
-    <format dxfId="4">
-      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
-        <references count="2">
-          <reference field="4294967294" count="1" selected="0">
-            <x v="2"/>
-          </reference>
-          <reference field="4" count="10">
-            <x v="1"/>
-            <x v="2"/>
-            <x v="3"/>
-            <x v="4"/>
-            <x v="5"/>
-            <x v="6"/>
-            <x v="7"/>
-            <x v="8"/>
-            <x v="9"/>
-            <x v="10"/>
           </reference>
         </references>
       </pivotArea>
@@ -7926,7 +7926,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC17F4EE-C40B-4E7F-A41C-76A7386395F3}">
   <dimension ref="A1:T74"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
       <selection activeCell="L2" sqref="L2"/>
     </sheetView>
   </sheetViews>
@@ -11447,7 +11447,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="81" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="V52" sqref="V52"/>
     </sheetView>
   </sheetViews>

</xml_diff>